<commit_message>
added columns to find min/max values.
</commit_message>
<xml_diff>
--- a/code/screpo/figures/results/comparison.xlsx
+++ b/code/screpo/figures/results/comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah4c20\Asyl\PostDoc\SOCIALCARE\code\screpo\outputs\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah4c20\Asyl\PostDoc\SOCIALCARE\code\screpo\figures\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ECE142-563F-4B38-8C56-B7FEF142B504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178E2681-0C53-4F04-90A4-13ED6742CAEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hampshire" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="64">
   <si>
     <t>Abicare</t>
   </si>
@@ -213,6 +213,18 @@
   <si>
     <t>Paper Osrm Best</t>
   </si>
+  <si>
+    <t>Diff Total Time</t>
+  </si>
+  <si>
+    <t>Diff Total Travel</t>
+  </si>
+  <si>
+    <t>Diff Total Wait</t>
+  </si>
+  <si>
+    <t>Diff DistJobs</t>
+  </si>
 </sst>
 </file>
 
@@ -367,7 +379,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +583,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -732,7 +750,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -777,6 +795,7 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="18" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1143,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ767"/>
+  <dimension ref="A1:BD767"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView topLeftCell="AD1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="BD4" sqref="BD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1209,7 @@
     <col min="49" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1376,8 +1395,20 @@
       <c r="AZ2" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>44137</v>
       </c>
@@ -1488,11 +1519,11 @@
         <v>391</v>
       </c>
       <c r="AK3" s="1" t="str">
-        <f>IF(I3&lt;Y3, "Abicare", "DST")</f>
+        <f t="shared" ref="AK3:AL9" si="0">IF(I3&lt;Y3, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AL3" s="1" t="str">
-        <f>IF(J3&lt;Z3, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM3" s="1" t="str">
@@ -1500,7 +1531,7 @@
         <v>DST</v>
       </c>
       <c r="AN3" s="1" t="str">
-        <f t="shared" ref="AN3:AN9" si="0">IF(L3&lt;AA3, "Abicare", "DST")</f>
+        <f t="shared" ref="AN3:AN9" si="1">IF(L3&lt;AA3, "Abicare", "DST")</f>
         <v>Abicare</v>
       </c>
       <c r="AO3" s="1" t="str">
@@ -1550,8 +1581,24 @@
         <f>IF(X3&gt;AG3, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA3" s="16">
+        <f>I3-Y3</f>
+        <v>187.53999999999996</v>
+      </c>
+      <c r="BB3" s="16">
+        <f>K3-Z3</f>
+        <v>140.602</v>
+      </c>
+      <c r="BC3" s="16">
+        <f>M3-AA3</f>
+        <v>46.937999999999874</v>
+      </c>
+      <c r="BD3" s="16">
+        <f>P3-AC3</f>
+        <v>127.09670000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>44138</v>
       </c>
@@ -1583,7 +1630,7 @@
         <v>1580.1166000000001</v>
       </c>
       <c r="M4" s="9">
-        <f t="shared" ref="M4:M9" si="1">I4-H4-K4</f>
+        <f t="shared" ref="M4:M9" si="2">I4-H4-K4</f>
         <v>1688.423</v>
       </c>
       <c r="N4" s="9">
@@ -1656,70 +1703,86 @@
         <v>334</v>
       </c>
       <c r="AK4" s="1" t="str">
-        <f>IF(I4&lt;Y4, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL4" s="1" t="str">
-        <f>IF(J4&lt;Z4, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM4" s="1" t="str">
-        <f t="shared" ref="AM4:AM9" si="2">IF(K4&lt;Z4, "AbiOSRM","DST")</f>
+        <f t="shared" ref="AM4:AM9" si="3">IF(K4&lt;Z4, "AbiOSRM","DST")</f>
         <v>DST</v>
       </c>
       <c r="AN4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO4" s="1" t="str">
-        <f t="shared" ref="AO4:AO9" si="3">IF(M4&lt;AA4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AO4:AO9" si="4">IF(M4&lt;AA4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AP4" s="8">
         <v>0</v>
       </c>
       <c r="AQ4" s="1" t="str">
-        <f t="shared" ref="AQ4:AQ9" si="4">IF(O4&lt;AC4, "Abicare","DST")</f>
+        <f t="shared" ref="AQ4:AQ9" si="5">IF(O4&lt;AC4, "Abicare","DST")</f>
         <v>DST</v>
       </c>
       <c r="AR4" s="1" t="str">
-        <f t="shared" ref="AR4:AR9" si="5">IF(P4&lt;AC4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AR4:AR9" si="6">IF(P4&lt;AC4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AS4" s="1" t="str">
-        <f t="shared" ref="AS4:AS9" si="6">IF(Q4&gt;AD4,"Abicare","DST")</f>
+        <f t="shared" ref="AS4:AS9" si="7">IF(Q4&gt;AD4,"Abicare","DST")</f>
         <v>DST</v>
       </c>
       <c r="AT4" s="1" t="str">
-        <f t="shared" ref="AT4:AT9" si="7">IF(R4&gt;AE4, "Abicare", "DST")</f>
+        <f t="shared" ref="AT4:AT9" si="8">IF(R4&gt;AE4, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AU4" s="1" t="str">
-        <f t="shared" ref="AU4:AU9" si="8">IF(S4&gt;AF4, "Abicare", "DST")</f>
+        <f t="shared" ref="AU4:AU9" si="9">IF(S4&gt;AF4, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AV4" s="1" t="str">
-        <f t="shared" ref="AV4:AV9" si="9">IF(T4&gt;AG4, "Abicare", "DST")</f>
+        <f t="shared" ref="AV4:AV9" si="10">IF(T4&gt;AG4, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AW4" s="1" t="str">
-        <f t="shared" ref="AW4:AW9" si="10">IF(U4&gt;AD4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AW4:AW9" si="11">IF(U4&gt;AD4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AX4" s="1" t="str">
-        <f t="shared" ref="AX4:AX9" si="11">IF(V4&gt;AE4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AX4:AX9" si="12">IF(V4&gt;AE4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AY4" s="1" t="str">
-        <f t="shared" ref="AY4:AY9" si="12">IF(W4&gt;AF4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AY4:AY9" si="13">IF(W4&gt;AF4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AZ4" s="1" t="str">
-        <f t="shared" ref="AZ4:AZ9" si="13">IF(X4&gt;AG4, "AbiOSRM", "DST")</f>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AZ4:AZ9" si="14">IF(X4&gt;AG4, "AbiOSRM", "DST")</f>
+        <v>DST</v>
+      </c>
+      <c r="BA4" s="16">
+        <f t="shared" ref="BA4:BA9" si="15">I4-Y4</f>
+        <v>177.31999999999971</v>
+      </c>
+      <c r="BB4" s="18">
+        <f t="shared" ref="BB4:BB9" si="16">K4-Z4</f>
+        <v>154.55699999999999</v>
+      </c>
+      <c r="BC4" s="16">
+        <f t="shared" ref="BC4:BC9" si="17">M4-AA4</f>
+        <v>22.772999999999911</v>
+      </c>
+      <c r="BD4" s="18">
+        <f t="shared" ref="BD4:BD9" si="18">P4-AC4</f>
+        <v>154.31989999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>44139</v>
       </c>
@@ -1751,7 +1814,7 @@
         <v>1189.2333000000001</v>
       </c>
       <c r="M5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1295.48</v>
       </c>
       <c r="N5" s="9">
@@ -1824,70 +1887,86 @@
         <v>332</v>
       </c>
       <c r="AK5" s="1" t="str">
-        <f>IF(I5&lt;Y5, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL5" s="1" t="str">
-        <f>IF(J5&lt;Z5, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>DST</v>
       </c>
       <c r="AN5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO5" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AP5" s="8">
         <v>0</v>
       </c>
       <c r="AQ5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AR5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AS5" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AT5" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AU5" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AV5" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>DST</v>
       </c>
       <c r="AW5" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>DST</v>
       </c>
       <c r="AX5" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DST</v>
       </c>
       <c r="AY5" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>DST</v>
       </c>
       <c r="AZ5" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>DST</v>
+      </c>
+      <c r="BA5" s="16">
+        <f t="shared" si="15"/>
+        <v>163.61999999999989</v>
+      </c>
+      <c r="BB5" s="16">
+        <f t="shared" si="16"/>
+        <v>141.93999999999997</v>
+      </c>
+      <c r="BC5" s="16">
+        <f t="shared" si="17"/>
+        <v>21.680000000000064</v>
+      </c>
+      <c r="BD5" s="16">
+        <f t="shared" si="18"/>
+        <v>135.95779999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>44140</v>
       </c>
@@ -1919,7 +1998,7 @@
         <v>1159.5833</v>
       </c>
       <c r="M6" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1260.0529999999999</v>
       </c>
       <c r="N6" s="9">
@@ -1992,70 +2071,86 @@
         <v>320</v>
       </c>
       <c r="AK6" s="1" t="str">
-        <f>IF(I6&lt;Y6, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL6" s="1" t="str">
-        <f>IF(J6&lt;Z6, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>DST</v>
       </c>
       <c r="AN6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO6" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AP6" s="8">
         <v>0</v>
       </c>
       <c r="AQ6" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AR6" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AS6" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AT6" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AU6" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AV6" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>DST</v>
       </c>
       <c r="AW6" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>DST</v>
       </c>
       <c r="AX6" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DST</v>
       </c>
       <c r="AY6" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>DST</v>
       </c>
       <c r="AZ6" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>DST</v>
+      </c>
+      <c r="BA6" s="16">
+        <f t="shared" si="15"/>
+        <v>175.27999999999975</v>
+      </c>
+      <c r="BB6" s="16">
+        <f t="shared" si="16"/>
+        <v>118.50700000000001</v>
+      </c>
+      <c r="BC6" s="16">
+        <f t="shared" si="17"/>
+        <v>56.772999999999911</v>
+      </c>
+      <c r="BD6" s="16">
+        <f t="shared" si="18"/>
+        <v>108.52790000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>44141</v>
       </c>
@@ -2087,7 +2182,7 @@
         <v>1065.5</v>
       </c>
       <c r="M7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1166.777</v>
       </c>
       <c r="N7" s="9">
@@ -2160,70 +2255,86 @@
         <v>288</v>
       </c>
       <c r="AK7" s="1" t="str">
-        <f>IF(I7&lt;Y7, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL7" s="1" t="str">
-        <f>IF(J7&lt;Z7, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>DST</v>
       </c>
       <c r="AN7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DST</v>
       </c>
       <c r="AO7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AP7" s="8">
         <v>0</v>
       </c>
       <c r="AQ7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AR7" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AS7" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AT7" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AU7" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AV7" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>DST</v>
       </c>
       <c r="AW7" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>DST</v>
       </c>
       <c r="AX7" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DST</v>
       </c>
       <c r="AY7" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>DST</v>
       </c>
       <c r="AZ7" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>DST</v>
+      </c>
+      <c r="BA7" s="18">
+        <f t="shared" si="15"/>
+        <v>257.64000000000033</v>
+      </c>
+      <c r="BB7" s="16">
+        <f t="shared" si="16"/>
+        <v>134.46300000000002</v>
+      </c>
+      <c r="BC7" s="18">
+        <f t="shared" si="17"/>
+        <v>123.17700000000013</v>
+      </c>
+      <c r="BD7" s="16">
+        <f t="shared" si="18"/>
+        <v>134.04940000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>44142</v>
       </c>
@@ -2255,7 +2366,7 @@
         <v>957.33299999999997</v>
       </c>
       <c r="M8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1053.172</v>
       </c>
       <c r="N8" s="9">
@@ -2328,70 +2439,86 @@
         <v>709</v>
       </c>
       <c r="AK8" s="1" t="str">
-        <f>IF(I8&lt;Y8, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL8" s="1" t="str">
-        <f>IF(J8&lt;Z8, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>DST</v>
       </c>
       <c r="AN8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO8" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AP8" s="8">
         <v>0</v>
       </c>
       <c r="AQ8" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AR8" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AS8" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AT8" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AU8" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AV8" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>DST</v>
       </c>
       <c r="AW8" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>DST</v>
       </c>
       <c r="AX8" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DST</v>
       </c>
       <c r="AY8" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>DST</v>
       </c>
       <c r="AZ8" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>DST</v>
+      </c>
+      <c r="BA8" s="16">
+        <f t="shared" si="15"/>
+        <v>163.65000000000009</v>
+      </c>
+      <c r="BB8" s="16">
+        <f t="shared" si="16"/>
+        <v>113.01799999999997</v>
+      </c>
+      <c r="BC8" s="16">
+        <f t="shared" si="17"/>
+        <v>50.632000000000062</v>
+      </c>
+      <c r="BD8" s="16">
+        <f t="shared" si="18"/>
+        <v>114.62340000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>44143</v>
       </c>
@@ -2423,7 +2550,7 @@
         <v>1019.59</v>
       </c>
       <c r="M9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1100.277</v>
       </c>
       <c r="N9" s="9">
@@ -2496,70 +2623,86 @@
         <v>664</v>
       </c>
       <c r="AK9" s="1" t="str">
-        <f>IF(I9&lt;Y9, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL9" s="1" t="str">
-        <f>IF(J9&lt;Z9, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>DST</v>
       </c>
       <c r="AN9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO9" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AP9" s="8">
         <v>0</v>
       </c>
       <c r="AQ9" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AR9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AS9" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AT9" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AU9" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AV9" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>DST</v>
       </c>
       <c r="AW9" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>DST</v>
       </c>
       <c r="AX9" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>DST</v>
       </c>
       <c r="AY9" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>DST</v>
       </c>
       <c r="AZ9" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="14"/>
+        <v>DST</v>
+      </c>
+      <c r="BA9" s="16">
+        <f t="shared" si="15"/>
+        <v>111.98999999999978</v>
+      </c>
+      <c r="BB9" s="16">
+        <f t="shared" si="16"/>
+        <v>101.04300000000001</v>
+      </c>
+      <c r="BC9" s="16">
+        <f t="shared" si="17"/>
+        <v>10.957000000000107</v>
+      </c>
+      <c r="BD9" s="16">
+        <f t="shared" si="18"/>
+        <v>90.665099999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -2597,7 +2740,7 @@
       <c r="AR10" s="10"/>
       <c r="AS10" s="10"/>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2638,8 +2781,24 @@
       <c r="AQ11" s="10"/>
       <c r="AR11" s="10"/>
       <c r="AS11" s="10"/>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA11" s="16">
+        <f>MAX(BA3:BA9)</f>
+        <v>257.64000000000033</v>
+      </c>
+      <c r="BB11" s="16">
+        <f>MAX(BB3:BB9)</f>
+        <v>154.55699999999999</v>
+      </c>
+      <c r="BC11" s="16">
+        <f>MAX(BC3:BC9)</f>
+        <v>123.17700000000013</v>
+      </c>
+      <c r="BD11" s="16">
+        <f>MAX(BD3:BD9)</f>
+        <v>154.31989999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -2677,7 +2836,7 @@
       <c r="AR12" s="10"/>
       <c r="AS12" s="10"/>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2715,18 +2874,18 @@
       <c r="AR13" s="10"/>
       <c r="AS13" s="10"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="M14" s="16"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="Q15" s="11"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -6518,10 +6677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1977999D-E23E-4C98-A23D-154E3F09823B}">
-  <dimension ref="A1:AZ767"/>
+  <dimension ref="A1:BD767"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AP30" sqref="AP30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6560,7 +6719,7 @@
     <col min="49" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -6583,7 +6742,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -6740,8 +6899,20 @@
       <c r="AZ2" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>44137</v>
       </c>
@@ -6852,11 +7023,11 @@
         <v>61</v>
       </c>
       <c r="AK3" s="1" t="str">
-        <f>IF(I3&lt;Y3, "Abicare", "DST")</f>
+        <f t="shared" ref="AK3:AL9" si="0">IF(I3&lt;Y3, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AL3" s="1" t="str">
-        <f>IF(J3&lt;Z3, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM3" s="1" t="str">
@@ -6864,7 +7035,7 @@
         <v>AbiOSRM</v>
       </c>
       <c r="AN3" s="1" t="str">
-        <f t="shared" ref="AN3:AN9" si="0">IF(L3&lt;AA3, "Abicare", "DST")</f>
+        <f t="shared" ref="AN3:AN9" si="1">IF(L3&lt;AA3, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AO3" s="1" t="str">
@@ -6887,15 +7058,15 @@
         <v>Abicare</v>
       </c>
       <c r="AT3" s="1" t="str">
-        <f>IF(R3&gt;AE3, "Abicare", "DST")</f>
+        <f t="shared" ref="AT3:AV9" si="2">IF(R3&gt;AE3, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AU3" s="1" t="str">
-        <f>IF(S3&gt;AF3, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>Abicare</v>
       </c>
       <c r="AV3" s="1" t="str">
-        <f>IF(T3&gt;AG3, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW3" s="1" t="str">
@@ -6914,8 +7085,24 @@
         <f>IF(X3&gt;AG3, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA3" s="18">
+        <f>I3-Y3</f>
+        <v>433.84000000000015</v>
+      </c>
+      <c r="BB3" s="16">
+        <f>K3-Z3</f>
+        <v>-12.538999999999987</v>
+      </c>
+      <c r="BC3" s="16">
+        <f>M3-AA3</f>
+        <v>446.37900000000002</v>
+      </c>
+      <c r="BD3" s="16">
+        <f>P3-AC3</f>
+        <v>-72.057000000000016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>44138</v>
       </c>
@@ -6944,7 +7131,7 @@
         <v>1026.3800000000001</v>
       </c>
       <c r="M4" s="9">
-        <f t="shared" ref="M4:M9" si="1">I4-H4-K4</f>
+        <f t="shared" ref="M4:M9" si="3">I4-H4-K4</f>
         <v>1079.1100000000001</v>
       </c>
       <c r="N4" s="9">
@@ -7017,895 +7204,991 @@
         <v>57</v>
       </c>
       <c r="AK4" s="1" t="str">
-        <f>IF(I4&lt;Y4, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL4" s="1" t="str">
-        <f>IF(J4&lt;Z4, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>Abicare</v>
       </c>
       <c r="AM4" s="1" t="str">
-        <f t="shared" ref="AM4:AM9" si="2">IF(K4&lt;Z4, "AbiOSRM","DST")</f>
+        <f t="shared" ref="AM4:AM9" si="4">IF(K4&lt;Z4, "AbiOSRM","DST")</f>
         <v>AbiOSRM</v>
       </c>
       <c r="AN4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DST</v>
       </c>
       <c r="AO4" s="1" t="str">
-        <f t="shared" ref="AO4:AO9" si="3">IF(M4&lt;AA4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AO4:AO9" si="5">IF(M4&lt;AA4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AP4" s="8">
         <v>0</v>
       </c>
       <c r="AQ4" s="1" t="str">
-        <f t="shared" ref="AQ4:AQ9" si="4">IF(O4&lt;AC4, "Abicare","DST")</f>
+        <f t="shared" ref="AQ4:AQ9" si="6">IF(O4&lt;AC4, "Abicare","DST")</f>
         <v>Abicare</v>
       </c>
       <c r="AR4" s="1" t="str">
-        <f t="shared" ref="AR4:AR9" si="5">IF(P4&lt;AC4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AR4:AR9" si="7">IF(P4&lt;AC4, "AbiOSRM", "DST")</f>
         <v>AbiOSRM</v>
       </c>
       <c r="AS4" s="1" t="str">
-        <f t="shared" ref="AS4:AS9" si="6">IF(Q4&gt;AD4,"Abicare","DST")</f>
+        <f t="shared" ref="AS4:AS9" si="8">IF(Q4&gt;AD4,"Abicare","DST")</f>
         <v>Abicare</v>
       </c>
       <c r="AT4" s="1" t="str">
-        <f>IF(R4&gt;AE4, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>Abicare</v>
       </c>
       <c r="AU4" s="1" t="str">
-        <f>IF(S4&gt;AF4, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>Abicare</v>
       </c>
       <c r="AV4" s="1" t="str">
-        <f>IF(T4&gt;AG4, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW4" s="1" t="str">
-        <f t="shared" ref="AW4:AZ9" si="7">IF(U4&gt;AD4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AW4:AZ9" si="9">IF(U4&gt;AD4, "AbiOSRM", "DST")</f>
         <v>AbiOSRM</v>
       </c>
       <c r="AX4" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AY4" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AZ4" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA4" s="16">
+        <f t="shared" ref="BA4:BA9" si="10">I4-Y4</f>
+        <v>271.30000000000018</v>
+      </c>
+      <c r="BB4" s="16">
+        <f t="shared" ref="BB4:BB9" si="11">K4-Z4</f>
+        <v>-69.990000000000009</v>
+      </c>
+      <c r="BC4" s="16">
+        <f t="shared" ref="BC4:BC9" si="12">M4-AA4</f>
+        <v>341.30000000000018</v>
+      </c>
+      <c r="BD4" s="16">
+        <f t="shared" ref="BD4:BD9" si="13">P4-AC4</f>
+        <v>-160.32090000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>44139</v>
+      </c>
+      <c r="E5" s="1">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
+        <v>105</v>
+      </c>
+      <c r="G5" s="1">
+        <v>39</v>
+      </c>
+      <c r="H5" s="13">
+        <v>4590</v>
+      </c>
+      <c r="I5" s="9">
+        <v>6135</v>
+      </c>
+      <c r="J5" s="9">
+        <v>769.78300000000002</v>
+      </c>
+      <c r="K5" s="9">
+        <v>722.41700000000003</v>
+      </c>
+      <c r="L5" s="9">
+        <v>775.21659999999997</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="3"/>
+        <v>822.58299999999997</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
+        <v>551.37090000000001</v>
+      </c>
+      <c r="P5" s="9">
+        <v>550.60199999999998</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>-230.9349</v>
+      </c>
+      <c r="R5" s="9">
+        <v>-256.59399999999999</v>
+      </c>
+      <c r="S5" s="9">
+        <v>-319.43490000000003</v>
+      </c>
+      <c r="T5" s="9">
+        <v>-1545</v>
+      </c>
+      <c r="U5" s="9">
+        <v>-216.72499999999999</v>
+      </c>
+      <c r="V5" s="9">
+        <v>-240.80600000000001</v>
+      </c>
+      <c r="W5" s="9">
+        <v>-305.22500000000002</v>
+      </c>
+      <c r="X5" s="9">
+        <v>-1545</v>
+      </c>
+      <c r="Y5" s="9">
+        <v>6044.82</v>
+      </c>
+      <c r="Z5" s="9">
+        <v>895.18</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>559.64</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>1452.1433</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>822.69849999999997</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>-467801.89</v>
+      </c>
+      <c r="AE5" s="9">
+        <v>-313.31</v>
+      </c>
+      <c r="AF5" s="9">
+        <v>-467891.16</v>
+      </c>
+      <c r="AG5" s="9">
+        <v>-1683.58</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="9">
+        <v>686.739779</v>
+      </c>
+      <c r="AJ5" s="10">
+        <v>46</v>
+      </c>
+      <c r="AK5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DST</v>
+      </c>
+      <c r="AL5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AM5" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AN5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DST</v>
+      </c>
+      <c r="AO5" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>DST</v>
+      </c>
+      <c r="AP5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AR5" s="1" t="str">
         <f t="shared" si="7"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AY4" s="1" t="str">
+      <c r="AS5" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AT5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AU5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AV5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AW5" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AX5" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AY5" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AZ5" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="BA5" s="16">
+        <f t="shared" si="10"/>
+        <v>90.180000000000291</v>
+      </c>
+      <c r="BB5" s="16">
+        <f t="shared" si="11"/>
+        <v>-172.76299999999992</v>
+      </c>
+      <c r="BC5" s="16">
+        <f t="shared" si="12"/>
+        <v>262.94299999999998</v>
+      </c>
+      <c r="BD5" s="16">
+        <f t="shared" si="13"/>
+        <v>-272.09649999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>44140</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>116</v>
+      </c>
+      <c r="G6" s="1">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13">
+        <v>4740</v>
+      </c>
+      <c r="I6" s="9">
+        <v>7200</v>
+      </c>
+      <c r="J6" s="9">
+        <v>798.19899999999996</v>
+      </c>
+      <c r="K6" s="9">
+        <v>745.85699999999997</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1661.7999</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="3"/>
+        <v>1714.143</v>
+      </c>
+      <c r="N6" s="9">
+        <v>0</v>
+      </c>
+      <c r="O6" s="9">
+        <v>573.44949999999994</v>
+      </c>
+      <c r="P6" s="9">
+        <v>561.89800000000002</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>-239.4599</v>
+      </c>
+      <c r="R6" s="9">
+        <v>-266.06599999999997</v>
+      </c>
+      <c r="S6" s="9">
+        <v>-327.96</v>
+      </c>
+      <c r="T6" s="9">
+        <v>-2459.9899999999998</v>
+      </c>
+      <c r="U6" s="9">
+        <v>-223.75700000000001</v>
+      </c>
+      <c r="V6" s="9">
+        <v>-248.619</v>
+      </c>
+      <c r="W6" s="9">
+        <v>-312.25700000000001</v>
+      </c>
+      <c r="X6" s="9">
+        <v>-2460</v>
+      </c>
+      <c r="Y6" s="9">
+        <v>6955.46</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>687.87</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>1527.59</v>
+      </c>
+      <c r="AB6" s="9">
+        <v>1416.8298</v>
+      </c>
+      <c r="AC6" s="9">
+        <v>578.19860000000006</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>-16839.689999999999</v>
+      </c>
+      <c r="AE6" s="9">
+        <v>-229.51</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>-16928.189999999999</v>
+      </c>
+      <c r="AG6" s="9">
+        <v>-2218.77</v>
+      </c>
+      <c r="AH6" s="10">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="9">
+        <v>717.74900000000002</v>
+      </c>
+      <c r="AJ6" s="10">
+        <v>35</v>
+      </c>
+      <c r="AK6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DST</v>
+      </c>
+      <c r="AL6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DST</v>
+      </c>
+      <c r="AM6" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>DST</v>
+      </c>
+      <c r="AN6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DST</v>
+      </c>
+      <c r="AO6" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>DST</v>
+      </c>
+      <c r="AP6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AR6" s="1" t="str">
         <f t="shared" si="7"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AZ4" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>44139</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="AS6" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AT6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>DST</v>
+      </c>
+      <c r="AU6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AV6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>DST</v>
+      </c>
+      <c r="AW6" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AX6" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="AY6" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AZ6" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA6" s="16">
+        <f t="shared" si="10"/>
+        <v>244.53999999999996</v>
+      </c>
+      <c r="BB6" s="18">
+        <f t="shared" si="11"/>
+        <v>57.986999999999966</v>
+      </c>
+      <c r="BC6" s="16">
+        <f t="shared" si="12"/>
+        <v>186.55300000000011</v>
+      </c>
+      <c r="BD6" s="18">
+        <f t="shared" si="13"/>
+        <v>-16.300600000000031</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>44141</v>
+      </c>
+      <c r="E7" s="1">
         <v>15</v>
       </c>
-      <c r="F5" s="1">
-        <v>105</v>
-      </c>
-      <c r="G5" s="1">
-        <v>39</v>
-      </c>
-      <c r="H5" s="13">
-        <v>4590</v>
-      </c>
-      <c r="I5" s="9">
-        <v>6135</v>
-      </c>
-      <c r="J5" s="9">
-        <v>769.78300000000002</v>
-      </c>
-      <c r="K5" s="9">
-        <v>722.41700000000003</v>
-      </c>
-      <c r="L5" s="9">
-        <v>775.21659999999997</v>
-      </c>
-      <c r="M5" s="9">
+      <c r="F7" s="1">
+        <v>114</v>
+      </c>
+      <c r="G7" s="1">
+        <v>41</v>
+      </c>
+      <c r="H7" s="13">
+        <v>5085</v>
+      </c>
+      <c r="I7" s="9">
+        <v>7455</v>
+      </c>
+      <c r="J7" s="9">
+        <v>864.51660000000004</v>
+      </c>
+      <c r="K7" s="9">
+        <v>824.72</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1505.4833000000001</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" si="3"/>
+        <v>1545.28</v>
+      </c>
+      <c r="N7" s="9">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9">
+        <v>641.91579999999999</v>
+      </c>
+      <c r="P7" s="9">
+        <v>639.98599999999999</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>-259.35498999999999</v>
+      </c>
+      <c r="R7" s="9">
+        <v>-288.17219999999998</v>
+      </c>
+      <c r="S7" s="9">
+        <v>-338.85499900000002</v>
+      </c>
+      <c r="T7" s="9">
+        <v>-2369.9989999999998</v>
+      </c>
+      <c r="U7" s="9">
+        <v>-247.416</v>
+      </c>
+      <c r="V7" s="9">
+        <v>-274.90699999999998</v>
+      </c>
+      <c r="W7" s="9">
+        <v>-326.916</v>
+      </c>
+      <c r="X7" s="9">
+        <v>-2370</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>7100.96</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>920.79</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>1095.1600000000001</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>1444.4348</v>
+      </c>
+      <c r="AC7" s="9">
+        <v>831.14279999999997</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>-137059.57</v>
+      </c>
+      <c r="AE7" s="9">
+        <v>-315.38</v>
+      </c>
+      <c r="AF7" s="9">
+        <v>-137139.09</v>
+      </c>
+      <c r="AG7" s="9">
+        <v>-2079.35</v>
+      </c>
+      <c r="AH7" s="10">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="9">
+        <v>705.19914029999995</v>
+      </c>
+      <c r="AJ7" s="10">
+        <v>38</v>
+      </c>
+      <c r="AK7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DST</v>
+      </c>
+      <c r="AL7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AM7" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AN7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>822.58299999999997</v>
-      </c>
-      <c r="N5" s="9">
+        <v>DST</v>
+      </c>
+      <c r="AO7" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>DST</v>
+      </c>
+      <c r="AP7" s="8">
         <v>0</v>
       </c>
-      <c r="O5" s="9">
-        <v>551.37090000000001</v>
-      </c>
-      <c r="P5" s="9">
-        <v>550.60199999999998</v>
-      </c>
-      <c r="Q5" s="9">
-        <v>-230.9349</v>
-      </c>
-      <c r="R5" s="9">
-        <v>-256.59399999999999</v>
-      </c>
-      <c r="S5" s="9">
-        <v>-319.43490000000003</v>
-      </c>
-      <c r="T5" s="9">
-        <v>-1545</v>
-      </c>
-      <c r="U5" s="9">
-        <v>-216.72499999999999</v>
-      </c>
-      <c r="V5" s="9">
-        <v>-240.80600000000001</v>
-      </c>
-      <c r="W5" s="9">
-        <v>-305.22500000000002</v>
-      </c>
-      <c r="X5" s="9">
-        <v>-1545</v>
-      </c>
-      <c r="Y5" s="9">
-        <v>6044.82</v>
-      </c>
-      <c r="Z5" s="9">
-        <v>895.18</v>
-      </c>
-      <c r="AA5" s="9">
-        <v>559.64</v>
-      </c>
-      <c r="AB5" s="9">
-        <v>1452.1433</v>
-      </c>
-      <c r="AC5" s="9">
-        <v>822.69849999999997</v>
-      </c>
-      <c r="AD5" s="9">
-        <v>-467801.89</v>
-      </c>
-      <c r="AE5" s="9">
-        <v>-313.31</v>
-      </c>
-      <c r="AF5" s="9">
-        <v>-467891.16</v>
-      </c>
-      <c r="AG5" s="9">
-        <v>-1683.58</v>
-      </c>
-      <c r="AH5" s="10">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="9">
-        <v>686.739779</v>
-      </c>
-      <c r="AJ5" s="10">
-        <v>46</v>
-      </c>
-      <c r="AK5" s="1" t="str">
-        <f>IF(I5&lt;Y5, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AL5" s="1" t="str">
-        <f>IF(J5&lt;Z5, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AM5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AN5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>DST</v>
-      </c>
-      <c r="AO5" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>DST</v>
-      </c>
-      <c r="AP5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AR5" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AS5" s="1" t="str">
+      <c r="AQ7" s="1" t="str">
         <f t="shared" si="6"/>
         <v>Abicare</v>
       </c>
-      <c r="AT5" s="1" t="str">
-        <f>IF(R5&gt;AE5, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AU5" s="1" t="str">
-        <f>IF(S5&gt;AF5, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AV5" s="1" t="str">
-        <f>IF(T5&gt;AG5, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AW5" s="1" t="str">
+      <c r="AR7" s="1" t="str">
         <f t="shared" si="7"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AX5" s="1" t="str">
+      <c r="AS7" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AT7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AU7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AV7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>DST</v>
+      </c>
+      <c r="AW7" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AX7" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AY7" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AZ7" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA7" s="16">
+        <f t="shared" si="10"/>
+        <v>354.03999999999996</v>
+      </c>
+      <c r="BB7" s="16">
+        <f t="shared" si="11"/>
+        <v>-96.069999999999936</v>
+      </c>
+      <c r="BC7" s="18">
+        <f t="shared" si="12"/>
+        <v>450.11999999999989</v>
+      </c>
+      <c r="BD7" s="16">
+        <f t="shared" si="13"/>
+        <v>-191.15679999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>44142</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1">
+        <v>99</v>
+      </c>
+      <c r="G8" s="1">
+        <v>37</v>
+      </c>
+      <c r="H8" s="13">
+        <v>3360</v>
+      </c>
+      <c r="I8" s="9">
+        <v>4845</v>
+      </c>
+      <c r="J8" s="9">
+        <v>694.06659999999999</v>
+      </c>
+      <c r="K8" s="9">
+        <v>661.49699999999996</v>
+      </c>
+      <c r="L8" s="9">
+        <v>790.93330000000003</v>
+      </c>
+      <c r="M8" s="9">
+        <f t="shared" si="3"/>
+        <v>823.50300000000004</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0</v>
+      </c>
+      <c r="O8" s="9">
+        <v>498.1225</v>
+      </c>
+      <c r="P8" s="9">
+        <v>503.89</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>-208.2199</v>
+      </c>
+      <c r="R8" s="9">
+        <v>-231.35550000000001</v>
+      </c>
+      <c r="S8" s="9">
+        <v>-274.21999</v>
+      </c>
+      <c r="T8" s="9">
+        <v>-1484.999</v>
+      </c>
+      <c r="U8" s="9">
+        <v>-198.44900000000001</v>
+      </c>
+      <c r="V8" s="9">
+        <v>-220.499</v>
+      </c>
+      <c r="W8" s="9">
+        <v>-264.44900000000001</v>
+      </c>
+      <c r="X8" s="9">
+        <v>-1485</v>
+      </c>
+      <c r="Y8" s="9">
+        <v>4574.79</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>779.27</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>435.51</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>1134.0248999999999</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>662.53610000000003</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>-136250.45000000001</v>
+      </c>
+      <c r="AE8" s="9">
+        <v>-268.16000000000003</v>
+      </c>
+      <c r="AF8" s="9">
+        <v>-136316.73000000001</v>
+      </c>
+      <c r="AG8" s="9">
+        <v>-1277.79</v>
+      </c>
+      <c r="AH8" s="10">
+        <v>5</v>
+      </c>
+      <c r="AI8" s="9">
+        <v>661.16577729999995</v>
+      </c>
+      <c r="AJ8" s="10">
+        <v>69</v>
+      </c>
+      <c r="AK8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DST</v>
+      </c>
+      <c r="AL8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AM8" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AN8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DST</v>
+      </c>
+      <c r="AO8" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>DST</v>
+      </c>
+      <c r="AP8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AR8" s="1" t="str">
         <f t="shared" si="7"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AY5" s="1" t="str">
+      <c r="AS8" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AT8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AU8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AV8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>DST</v>
+      </c>
+      <c r="AW8" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AX8" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AY8" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AZ8" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA8" s="16">
+        <f t="shared" si="10"/>
+        <v>270.21000000000004</v>
+      </c>
+      <c r="BB8" s="16">
+        <f t="shared" si="11"/>
+        <v>-117.77300000000002</v>
+      </c>
+      <c r="BC8" s="16">
+        <f t="shared" si="12"/>
+        <v>387.99300000000005</v>
+      </c>
+      <c r="BD8" s="16">
+        <f t="shared" si="13"/>
+        <v>-158.64610000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>44143</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
+        <v>96</v>
+      </c>
+      <c r="G9" s="1">
+        <v>34</v>
+      </c>
+      <c r="H9" s="13">
+        <v>3255</v>
+      </c>
+      <c r="I9" s="9">
+        <v>4470</v>
+      </c>
+      <c r="J9" s="9">
+        <v>666.16600000000005</v>
+      </c>
+      <c r="K9" s="9">
+        <v>636.06700000000001</v>
+      </c>
+      <c r="L9" s="9">
+        <v>548.83330000000001</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" si="3"/>
+        <v>578.93299999999999</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <v>480.38920000000002</v>
+      </c>
+      <c r="P9" s="9">
+        <v>489.50700000000001</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>-199.84989999999999</v>
+      </c>
+      <c r="R9" s="9">
+        <v>-222.05500000000001</v>
+      </c>
+      <c r="S9" s="9">
+        <v>-249.34989999999999</v>
+      </c>
+      <c r="T9" s="9">
+        <v>-1215</v>
+      </c>
+      <c r="U9" s="9">
+        <v>-190.82</v>
+      </c>
+      <c r="V9" s="9">
+        <v>-212.02199999999999</v>
+      </c>
+      <c r="W9" s="9">
+        <v>-240.32</v>
+      </c>
+      <c r="X9" s="9">
+        <v>-1215</v>
+      </c>
+      <c r="Y9" s="9">
+        <v>4380.78</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>802.96</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>322.82</v>
+      </c>
+      <c r="AB9" s="9">
+        <v>1041.989</v>
+      </c>
+      <c r="AC9" s="9">
+        <v>676.26179999999999</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>-334907.56</v>
+      </c>
+      <c r="AE9" s="9">
+        <v>-280.94</v>
+      </c>
+      <c r="AF9" s="9">
+        <v>-334957.59999999998</v>
+      </c>
+      <c r="AG9" s="9">
+        <v>-1288.1099999999999</v>
+      </c>
+      <c r="AH9" s="10">
+        <v>5</v>
+      </c>
+      <c r="AI9" s="9">
+        <v>648.61416350000002</v>
+      </c>
+      <c r="AJ9" s="10">
+        <v>97</v>
+      </c>
+      <c r="AK9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DST</v>
+      </c>
+      <c r="AL9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AM9" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AbiOSRM</v>
+      </c>
+      <c r="AN9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>DST</v>
+      </c>
+      <c r="AO9" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>DST</v>
+      </c>
+      <c r="AP9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AR9" s="1" t="str">
         <f t="shared" si="7"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AZ5" s="1" t="str">
-        <f t="shared" si="7"/>
+      <c r="AS9" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AT9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AU9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AV9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Abicare</v>
+      </c>
+      <c r="AW9" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>AbiOSRM</v>
       </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>44140</v>
-      </c>
-      <c r="E6" s="1">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1">
-        <v>116</v>
-      </c>
-      <c r="G6" s="1">
-        <v>40</v>
-      </c>
-      <c r="H6" s="13">
-        <v>4740</v>
-      </c>
-      <c r="I6" s="9">
-        <v>7200</v>
-      </c>
-      <c r="J6" s="9">
-        <v>798.19899999999996</v>
-      </c>
-      <c r="K6" s="9">
-        <v>745.85699999999997</v>
-      </c>
-      <c r="L6" s="9">
-        <v>1661.7999</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="shared" si="1"/>
-        <v>1714.143</v>
-      </c>
-      <c r="N6" s="9">
-        <v>0</v>
-      </c>
-      <c r="O6" s="9">
-        <v>573.44949999999994</v>
-      </c>
-      <c r="P6" s="9">
-        <v>561.89800000000002</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>-239.4599</v>
-      </c>
-      <c r="R6" s="9">
-        <v>-266.06599999999997</v>
-      </c>
-      <c r="S6" s="9">
-        <v>-327.96</v>
-      </c>
-      <c r="T6" s="9">
-        <v>-2459.9899999999998</v>
-      </c>
-      <c r="U6" s="9">
-        <v>-223.75700000000001</v>
-      </c>
-      <c r="V6" s="9">
-        <v>-248.619</v>
-      </c>
-      <c r="W6" s="9">
-        <v>-312.25700000000001</v>
-      </c>
-      <c r="X6" s="9">
-        <v>-2460</v>
-      </c>
-      <c r="Y6" s="9">
-        <v>6955.46</v>
-      </c>
-      <c r="Z6" s="9">
-        <v>687.87</v>
-      </c>
-      <c r="AA6" s="9">
-        <v>1527.59</v>
-      </c>
-      <c r="AB6" s="9">
-        <v>1416.8298</v>
-      </c>
-      <c r="AC6" s="9">
-        <v>578.19860000000006</v>
-      </c>
-      <c r="AD6" s="9">
-        <v>-16839.689999999999</v>
-      </c>
-      <c r="AE6" s="9">
-        <v>-229.51</v>
-      </c>
-      <c r="AF6" s="9">
-        <v>-16928.189999999999</v>
-      </c>
-      <c r="AG6" s="9">
-        <v>-2218.77</v>
-      </c>
-      <c r="AH6" s="10">
-        <v>5</v>
-      </c>
-      <c r="AI6" s="9">
-        <v>717.74900000000002</v>
-      </c>
-      <c r="AJ6" s="10">
-        <v>35</v>
-      </c>
-      <c r="AK6" s="1" t="str">
-        <f>IF(I6&lt;Y6, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AL6" s="1" t="str">
-        <f>IF(J6&lt;Z6, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AM6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>DST</v>
-      </c>
-      <c r="AN6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>DST</v>
-      </c>
-      <c r="AO6" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>DST</v>
-      </c>
-      <c r="AP6" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AR6" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="AX9" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AS6" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AT6" s="1" t="str">
-        <f>IF(R6&gt;AE6, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AU6" s="1" t="str">
-        <f>IF(S6&gt;AF6, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AV6" s="1" t="str">
-        <f>IF(T6&gt;AG6, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AW6" s="1" t="str">
-        <f t="shared" si="7"/>
+      <c r="AY9" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AX6" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-      <c r="AY6" s="1" t="str">
-        <f t="shared" si="7"/>
+      <c r="AZ9" s="1" t="str">
+        <f t="shared" si="9"/>
         <v>AbiOSRM</v>
       </c>
-      <c r="AZ6" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>44141</v>
-      </c>
-      <c r="E7" s="1">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1">
-        <v>114</v>
-      </c>
-      <c r="G7" s="1">
-        <v>41</v>
-      </c>
-      <c r="H7" s="13">
-        <v>5085</v>
-      </c>
-      <c r="I7" s="9">
-        <v>7455</v>
-      </c>
-      <c r="J7" s="9">
-        <v>864.51660000000004</v>
-      </c>
-      <c r="K7" s="9">
-        <v>824.72</v>
-      </c>
-      <c r="L7" s="9">
-        <v>1505.4833000000001</v>
-      </c>
-      <c r="M7" s="9">
-        <f t="shared" si="1"/>
-        <v>1545.28</v>
-      </c>
-      <c r="N7" s="9">
-        <v>0</v>
-      </c>
-      <c r="O7" s="9">
-        <v>641.91579999999999</v>
-      </c>
-      <c r="P7" s="9">
-        <v>639.98599999999999</v>
-      </c>
-      <c r="Q7" s="9">
-        <v>-259.35498999999999</v>
-      </c>
-      <c r="R7" s="9">
-        <v>-288.17219999999998</v>
-      </c>
-      <c r="S7" s="9">
-        <v>-338.85499900000002</v>
-      </c>
-      <c r="T7" s="9">
-        <v>-2369.9989999999998</v>
-      </c>
-      <c r="U7" s="9">
-        <v>-247.416</v>
-      </c>
-      <c r="V7" s="9">
-        <v>-274.90699999999998</v>
-      </c>
-      <c r="W7" s="9">
-        <v>-326.916</v>
-      </c>
-      <c r="X7" s="9">
-        <v>-2370</v>
-      </c>
-      <c r="Y7" s="9">
-        <v>7100.96</v>
-      </c>
-      <c r="Z7" s="9">
-        <v>920.79</v>
-      </c>
-      <c r="AA7" s="9">
-        <v>1095.1600000000001</v>
-      </c>
-      <c r="AB7" s="9">
-        <v>1444.4348</v>
-      </c>
-      <c r="AC7" s="9">
-        <v>831.14279999999997</v>
-      </c>
-      <c r="AD7" s="9">
-        <v>-137059.57</v>
-      </c>
-      <c r="AE7" s="9">
-        <v>-315.38</v>
-      </c>
-      <c r="AF7" s="9">
-        <v>-137139.09</v>
-      </c>
-      <c r="AG7" s="9">
-        <v>-2079.35</v>
-      </c>
-      <c r="AH7" s="10">
-        <v>5</v>
-      </c>
-      <c r="AI7" s="9">
-        <v>705.19914029999995</v>
-      </c>
-      <c r="AJ7" s="10">
-        <v>38</v>
-      </c>
-      <c r="AK7" s="1" t="str">
-        <f>IF(I7&lt;Y7, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AL7" s="1" t="str">
-        <f>IF(J7&lt;Z7, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AM7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AN7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>DST</v>
-      </c>
-      <c r="AO7" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>DST</v>
-      </c>
-      <c r="AP7" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AR7" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AS7" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AT7" s="1" t="str">
-        <f>IF(R7&gt;AE7, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AU7" s="1" t="str">
-        <f>IF(S7&gt;AF7, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AV7" s="1" t="str">
-        <f>IF(T7&gt;AG7, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AW7" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AX7" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AY7" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AZ7" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>44142</v>
-      </c>
-      <c r="E8" s="1">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1">
-        <v>99</v>
-      </c>
-      <c r="G8" s="1">
-        <v>37</v>
-      </c>
-      <c r="H8" s="13">
-        <v>3360</v>
-      </c>
-      <c r="I8" s="9">
-        <v>4845</v>
-      </c>
-      <c r="J8" s="9">
-        <v>694.06659999999999</v>
-      </c>
-      <c r="K8" s="9">
-        <v>661.49699999999996</v>
-      </c>
-      <c r="L8" s="9">
-        <v>790.93330000000003</v>
-      </c>
-      <c r="M8" s="9">
-        <f t="shared" si="1"/>
-        <v>823.50300000000004</v>
-      </c>
-      <c r="N8" s="9">
-        <v>0</v>
-      </c>
-      <c r="O8" s="9">
-        <v>498.1225</v>
-      </c>
-      <c r="P8" s="9">
-        <v>503.89</v>
-      </c>
-      <c r="Q8" s="9">
-        <v>-208.2199</v>
-      </c>
-      <c r="R8" s="9">
-        <v>-231.35550000000001</v>
-      </c>
-      <c r="S8" s="9">
-        <v>-274.21999</v>
-      </c>
-      <c r="T8" s="9">
-        <v>-1484.999</v>
-      </c>
-      <c r="U8" s="9">
-        <v>-198.44900000000001</v>
-      </c>
-      <c r="V8" s="9">
-        <v>-220.499</v>
-      </c>
-      <c r="W8" s="9">
-        <v>-264.44900000000001</v>
-      </c>
-      <c r="X8" s="9">
-        <v>-1485</v>
-      </c>
-      <c r="Y8" s="9">
-        <v>4574.79</v>
-      </c>
-      <c r="Z8" s="9">
-        <v>779.27</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>435.51</v>
-      </c>
-      <c r="AB8" s="9">
-        <v>1134.0248999999999</v>
-      </c>
-      <c r="AC8" s="9">
-        <v>662.53610000000003</v>
-      </c>
-      <c r="AD8" s="9">
-        <v>-136250.45000000001</v>
-      </c>
-      <c r="AE8" s="9">
-        <v>-268.16000000000003</v>
-      </c>
-      <c r="AF8" s="9">
-        <v>-136316.73000000001</v>
-      </c>
-      <c r="AG8" s="9">
-        <v>-1277.79</v>
-      </c>
-      <c r="AH8" s="10">
-        <v>5</v>
-      </c>
-      <c r="AI8" s="9">
-        <v>661.16577729999995</v>
-      </c>
-      <c r="AJ8" s="10">
-        <v>69</v>
-      </c>
-      <c r="AK8" s="1" t="str">
-        <f>IF(I8&lt;Y8, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AL8" s="1" t="str">
-        <f>IF(J8&lt;Z8, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AM8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AN8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>DST</v>
-      </c>
-      <c r="AO8" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>DST</v>
-      </c>
-      <c r="AP8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AR8" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AS8" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AT8" s="1" t="str">
-        <f>IF(R8&gt;AE8, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AU8" s="1" t="str">
-        <f>IF(S8&gt;AF8, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AV8" s="1" t="str">
-        <f>IF(T8&gt;AG8, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AW8" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AX8" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AY8" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AZ8" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>44143</v>
-      </c>
-      <c r="E9" s="1">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1">
-        <v>96</v>
-      </c>
-      <c r="G9" s="1">
-        <v>34</v>
-      </c>
-      <c r="H9" s="13">
-        <v>3255</v>
-      </c>
-      <c r="I9" s="9">
-        <v>4470</v>
-      </c>
-      <c r="J9" s="9">
-        <v>666.16600000000005</v>
-      </c>
-      <c r="K9" s="9">
-        <v>636.06700000000001</v>
-      </c>
-      <c r="L9" s="9">
-        <v>548.83330000000001</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" si="1"/>
-        <v>578.93299999999999</v>
-      </c>
-      <c r="N9" s="9">
-        <v>0</v>
-      </c>
-      <c r="O9" s="9">
-        <v>480.38920000000002</v>
-      </c>
-      <c r="P9" s="9">
-        <v>489.50700000000001</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>-199.84989999999999</v>
-      </c>
-      <c r="R9" s="9">
-        <v>-222.05500000000001</v>
-      </c>
-      <c r="S9" s="9">
-        <v>-249.34989999999999</v>
-      </c>
-      <c r="T9" s="9">
-        <v>-1215</v>
-      </c>
-      <c r="U9" s="9">
-        <v>-190.82</v>
-      </c>
-      <c r="V9" s="9">
-        <v>-212.02199999999999</v>
-      </c>
-      <c r="W9" s="9">
-        <v>-240.32</v>
-      </c>
-      <c r="X9" s="9">
-        <v>-1215</v>
-      </c>
-      <c r="Y9" s="9">
-        <v>4380.78</v>
-      </c>
-      <c r="Z9" s="9">
-        <v>802.96</v>
-      </c>
-      <c r="AA9" s="9">
-        <v>322.82</v>
-      </c>
-      <c r="AB9" s="9">
-        <v>1041.989</v>
-      </c>
-      <c r="AC9" s="9">
-        <v>676.26179999999999</v>
-      </c>
-      <c r="AD9" s="9">
-        <v>-334907.56</v>
-      </c>
-      <c r="AE9" s="9">
-        <v>-280.94</v>
-      </c>
-      <c r="AF9" s="9">
-        <v>-334957.59999999998</v>
-      </c>
-      <c r="AG9" s="9">
-        <v>-1288.1099999999999</v>
-      </c>
-      <c r="AH9" s="10">
-        <v>5</v>
-      </c>
-      <c r="AI9" s="9">
-        <v>648.61416350000002</v>
-      </c>
-      <c r="AJ9" s="10">
-        <v>97</v>
-      </c>
-      <c r="AK9" s="1" t="str">
-        <f>IF(I9&lt;Y9, "Abicare", "DST")</f>
-        <v>DST</v>
-      </c>
-      <c r="AL9" s="1" t="str">
-        <f>IF(J9&lt;Z9, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AM9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AN9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>DST</v>
-      </c>
-      <c r="AO9" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>DST</v>
-      </c>
-      <c r="AP9" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AR9" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AS9" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>Abicare</v>
-      </c>
-      <c r="AT9" s="1" t="str">
-        <f>IF(R9&gt;AE9, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AU9" s="1" t="str">
-        <f>IF(S9&gt;AF9, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AV9" s="1" t="str">
-        <f>IF(T9&gt;AG9, "Abicare", "DST")</f>
-        <v>Abicare</v>
-      </c>
-      <c r="AW9" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AX9" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AY9" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-      <c r="AZ9" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>AbiOSRM</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA9" s="16">
+        <f t="shared" si="10"/>
+        <v>89.220000000000255</v>
+      </c>
+      <c r="BB9" s="16">
+        <f t="shared" si="11"/>
+        <v>-166.89300000000003</v>
+      </c>
+      <c r="BC9" s="16">
+        <f t="shared" si="12"/>
+        <v>256.113</v>
+      </c>
+      <c r="BD9" s="16">
+        <f t="shared" si="13"/>
+        <v>-186.75479999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="10"/>
@@ -7945,7 +8228,7 @@
       <c r="AR10" s="10"/>
       <c r="AS10" s="10"/>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -7988,8 +8271,24 @@
       <c r="AQ11" s="10"/>
       <c r="AR11" s="10"/>
       <c r="AS11" s="10"/>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA11" s="16">
+        <f>MAX(BA3:BA9)</f>
+        <v>433.84000000000015</v>
+      </c>
+      <c r="BB11" s="16">
+        <f>MAX(BB3:BB9)</f>
+        <v>57.986999999999966</v>
+      </c>
+      <c r="BC11" s="16">
+        <f>MAX(BC3:BC9)</f>
+        <v>450.11999999999989</v>
+      </c>
+      <c r="BD11" s="16">
+        <f>MAX(BD3:BD9)</f>
+        <v>-16.300600000000031</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="H12" s="13"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -8028,7 +8327,7 @@
       <c r="AR12" s="10"/>
       <c r="AS12" s="10"/>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -8066,17 +8365,17 @@
       <c r="AR13" s="10"/>
       <c r="AS13" s="10"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="Q14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="Q15" s="11"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -11867,10 +12166,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49B5B4B-4533-44D7-8358-A79D8B3FBA76}">
-  <dimension ref="A1:AZ767"/>
+  <dimension ref="A1:BD767"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="BB17" sqref="BB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11906,7 +12205,7 @@
     <col min="49" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -11929,7 +12228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -12086,8 +12385,20 @@
       <c r="AZ2" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>44137</v>
       </c>
@@ -12198,11 +12509,11 @@
         <v>32717</v>
       </c>
       <c r="AK3" s="1" t="str">
-        <f>IF(I3&lt;Y3, "Abicare", "DST")</f>
+        <f t="shared" ref="AK3:AL9" si="0">IF(I3&lt;Y3, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AL3" s="1" t="str">
-        <f>IF(J3&lt;Z3, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM3" s="1" t="str">
@@ -12210,7 +12521,7 @@
         <v>DST</v>
       </c>
       <c r="AN3" s="1" t="str">
-        <f t="shared" ref="AN3:AN9" si="0">IF(L3&lt;AA3, "Abicare", "DST")</f>
+        <f t="shared" ref="AN3:AN9" si="1">IF(L3&lt;AA3, "Abicare", "DST")</f>
         <v>Abicare</v>
       </c>
       <c r="AO3" s="1" t="str">
@@ -12233,15 +12544,15 @@
         <v>DST</v>
       </c>
       <c r="AT3" s="1" t="str">
-        <f>IF(R3&gt;AE3, "Abicare", "DST")</f>
+        <f t="shared" ref="AT3:AV9" si="2">IF(R3&gt;AE3, "Abicare", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AU3" s="1" t="str">
-        <f>IF(S3&gt;AF3, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV3" s="1" t="str">
-        <f>IF(T3&gt;AG3, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW3" s="1" t="str">
@@ -12260,8 +12571,24 @@
         <f>IF(X3&gt;AG3, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA3" s="16">
+        <f>I3-Y3</f>
+        <v>30.099999999999909</v>
+      </c>
+      <c r="BB3" s="16">
+        <f>K3-Z3</f>
+        <v>28.236999999999995</v>
+      </c>
+      <c r="BC3" s="16">
+        <f>M3-AA3</f>
+        <v>1.8629999999999995</v>
+      </c>
+      <c r="BD3" s="16">
+        <f>P3-AC3</f>
+        <v>27.139699999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>44138</v>
       </c>
@@ -12290,7 +12617,7 @@
         <v>73.948999999999998</v>
       </c>
       <c r="M4" s="9">
-        <f t="shared" ref="M4:M9" si="1">I4-H4-K4</f>
+        <f t="shared" ref="M4:M9" si="3">I4-H4-K4</f>
         <v>110.53299999999999</v>
       </c>
       <c r="N4" s="9">
@@ -12363,70 +12690,86 @@
         <v>27561</v>
       </c>
       <c r="AK4" s="1" t="str">
-        <f>IF(I4&lt;Y4, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL4" s="1" t="str">
-        <f>IF(J4&lt;Z4, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM4" s="1" t="str">
-        <f t="shared" ref="AM4:AM9" si="2">IF(K4&lt;Z4, "AbiOSRM","DST")</f>
+        <f t="shared" ref="AM4:AM9" si="4">IF(K4&lt;Z4, "AbiOSRM","DST")</f>
         <v>DST</v>
       </c>
       <c r="AN4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DST</v>
       </c>
       <c r="AO4" s="1" t="str">
-        <f t="shared" ref="AO4:AO9" si="3">IF(M4&lt;AA4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AO4:AO9" si="5">IF(M4&lt;AA4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AP4" s="8">
         <v>0</v>
       </c>
       <c r="AQ4" s="1" t="str">
-        <f t="shared" ref="AQ4:AQ9" si="4">IF(O4&lt;AC4, "Abicare","DST")</f>
+        <f t="shared" ref="AQ4:AQ9" si="6">IF(O4&lt;AC4, "Abicare","DST")</f>
         <v>DST</v>
       </c>
       <c r="AR4" s="1" t="str">
-        <f t="shared" ref="AR4:AR9" si="5">IF(P4&lt;AC4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AR4:AR9" si="7">IF(P4&lt;AC4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AS4" s="1" t="str">
-        <f t="shared" ref="AS4:AS9" si="6">IF(Q4&gt;AD4,"Abicare","DST")</f>
+        <f t="shared" ref="AS4:AS9" si="8">IF(Q4&gt;AD4,"Abicare","DST")</f>
         <v>DST</v>
       </c>
       <c r="AT4" s="1" t="str">
-        <f>IF(R4&gt;AE4, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AU4" s="1" t="str">
-        <f>IF(S4&gt;AF4, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV4" s="1" t="str">
-        <f>IF(T4&gt;AG4, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW4" s="1" t="str">
-        <f t="shared" ref="AW4:AZ9" si="7">IF(U4&gt;AD4, "AbiOSRM", "DST")</f>
+        <f t="shared" ref="AW4:AZ9" si="9">IF(U4&gt;AD4, "AbiOSRM", "DST")</f>
         <v>DST</v>
       </c>
       <c r="AX4" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AY4" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AZ4" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA4" s="16">
+        <f t="shared" ref="BA4:BA9" si="10">I4-Y4</f>
+        <v>64.259999999999991</v>
+      </c>
+      <c r="BB4" s="16">
+        <f t="shared" ref="BB4:BB9" si="11">K4-Z4</f>
+        <v>10.257000000000019</v>
+      </c>
+      <c r="BC4" s="16">
+        <f t="shared" ref="BC4:BC9" si="12">M4-AA4</f>
+        <v>54.002999999999986</v>
+      </c>
+      <c r="BD4" s="16">
+        <f t="shared" ref="BD4:BD9" si="13">P4-AC4</f>
+        <v>7.3830000000000098</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>44139</v>
       </c>
@@ -12455,7 +12798,7 @@
         <v>36.716000000000001</v>
       </c>
       <c r="M5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>73.807999999999993</v>
       </c>
       <c r="N5" s="9">
@@ -12528,70 +12871,86 @@
         <v>16121</v>
       </c>
       <c r="AK5" s="1" t="str">
-        <f>IF(I5&lt;Y5, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL5" s="1" t="str">
-        <f>IF(J5&lt;Z5, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AN5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO5" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AP5" s="8">
         <v>0</v>
       </c>
       <c r="AQ5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AR5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AS5" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AT5" s="1" t="str">
-        <f>IF(R5&gt;AE5, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AU5" s="1" t="str">
-        <f>IF(S5&gt;AF5, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV5" s="1" t="str">
-        <f>IF(T5&gt;AG5, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW5" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AX5" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AY5" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AZ5" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA5" s="16">
+        <f t="shared" si="10"/>
+        <v>33.680000000000064</v>
+      </c>
+      <c r="BB5" s="16">
+        <f t="shared" si="11"/>
+        <v>21.402000000000001</v>
+      </c>
+      <c r="BC5" s="16">
+        <f t="shared" si="12"/>
+        <v>12.277999999999992</v>
+      </c>
+      <c r="BD5" s="16">
+        <f t="shared" si="13"/>
+        <v>17.896500000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>44140</v>
       </c>
@@ -12620,7 +12979,7 @@
         <v>338.416</v>
       </c>
       <c r="M6" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381.00700000000001</v>
       </c>
       <c r="N6" s="9">
@@ -12693,70 +13052,86 @@
         <v>15930</v>
       </c>
       <c r="AK6" s="1" t="str">
-        <f>IF(I6&lt;Y6, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL6" s="1" t="str">
-        <f>IF(J6&lt;Z6, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AN6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DST</v>
       </c>
       <c r="AO6" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AP6" s="8">
         <v>0</v>
       </c>
       <c r="AQ6" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AR6" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AS6" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AT6" s="1" t="str">
-        <f>IF(R6&gt;AE6, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AU6" s="1" t="str">
-        <f>IF(S6&gt;AF6, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV6" s="1" t="str">
-        <f>IF(T6&gt;AG6, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW6" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AX6" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AY6" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AZ6" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA6" s="16">
+        <f t="shared" si="10"/>
+        <v>95</v>
+      </c>
+      <c r="BB6" s="18">
+        <f t="shared" si="11"/>
+        <v>46.242999999999995</v>
+      </c>
+      <c r="BC6" s="16">
+        <f t="shared" si="12"/>
+        <v>48.757000000000005</v>
+      </c>
+      <c r="BD6" s="18">
+        <f t="shared" si="13"/>
+        <v>37.569100000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>44141</v>
       </c>
@@ -12785,7 +13160,7 @@
         <v>402.03300000000002</v>
       </c>
       <c r="M7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>431.92</v>
       </c>
       <c r="N7" s="9">
@@ -12858,70 +13233,86 @@
         <v>20125</v>
       </c>
       <c r="AK7" s="1" t="str">
-        <f>IF(I7&lt;Y7, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL7" s="1" t="str">
-        <f>IF(J7&lt;Z7, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AN7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>DST</v>
       </c>
       <c r="AO7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AP7" s="8">
         <v>0</v>
       </c>
       <c r="AQ7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AR7" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AS7" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AT7" s="1" t="str">
-        <f>IF(R7&gt;AE7, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AU7" s="1" t="str">
-        <f>IF(S7&gt;AF7, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV7" s="1" t="str">
-        <f>IF(T7&gt;AG7, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW7" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AX7" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AY7" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AZ7" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA7" s="18">
+        <f t="shared" si="10"/>
+        <v>124.72000000000003</v>
+      </c>
+      <c r="BB7" s="16">
+        <f t="shared" si="11"/>
+        <v>14.969999999999999</v>
+      </c>
+      <c r="BC7" s="18">
+        <f t="shared" si="12"/>
+        <v>109.75</v>
+      </c>
+      <c r="BD7" s="16">
+        <f t="shared" si="13"/>
+        <v>14.407599999999988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>44142</v>
       </c>
@@ -12950,7 +13341,7 @@
         <v>212.29900000000001</v>
       </c>
       <c r="M8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>246.08799999999999</v>
       </c>
       <c r="N8" s="9">
@@ -13023,70 +13414,86 @@
         <v>48046</v>
       </c>
       <c r="AK8" s="1" t="str">
-        <f>IF(I8&lt;Y8, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL8" s="1" t="str">
-        <f>IF(J8&lt;Z8, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AN8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO8" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AP8" s="8">
         <v>0</v>
       </c>
       <c r="AQ8" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AR8" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AS8" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AT8" s="1" t="str">
-        <f>IF(R8&gt;AE8, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AU8" s="1" t="str">
-        <f>IF(S8&gt;AF8, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV8" s="1" t="str">
-        <f>IF(T8&gt;AG8, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW8" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AX8" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AY8" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AZ8" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA8" s="16">
+        <f t="shared" si="10"/>
+        <v>59.080000000000041</v>
+      </c>
+      <c r="BB8" s="16">
+        <f t="shared" si="11"/>
+        <v>25.832000000000008</v>
+      </c>
+      <c r="BC8" s="16">
+        <f t="shared" si="12"/>
+        <v>33.24799999999999</v>
+      </c>
+      <c r="BD8" s="16">
+        <f t="shared" si="13"/>
+        <v>27.784599999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>44143</v>
       </c>
@@ -13115,7 +13522,7 @@
         <v>143.51660000000001</v>
       </c>
       <c r="M9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>177.405</v>
       </c>
       <c r="N9" s="9">
@@ -13188,70 +13595,86 @@
         <v>44925</v>
       </c>
       <c r="AK9" s="1" t="str">
-        <f>IF(I9&lt;Y9, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AL9" s="1" t="str">
-        <f>IF(J9&lt;Z9, "Abicare", "DST")</f>
+        <f t="shared" si="0"/>
         <v>DST</v>
       </c>
       <c r="AM9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>DST</v>
       </c>
       <c r="AN9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abicare</v>
       </c>
       <c r="AO9" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>DST</v>
       </c>
       <c r="AP9" s="8">
         <v>0</v>
       </c>
       <c r="AQ9" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>DST</v>
       </c>
       <c r="AR9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>DST</v>
       </c>
       <c r="AS9" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>DST</v>
       </c>
       <c r="AT9" s="1" t="str">
-        <f>IF(R9&gt;AE9, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AU9" s="1" t="str">
-        <f>IF(S9&gt;AF9, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AV9" s="1" t="str">
-        <f>IF(T9&gt;AG9, "Abicare", "DST")</f>
+        <f t="shared" si="2"/>
         <v>DST</v>
       </c>
       <c r="AW9" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AX9" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AY9" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>DST</v>
       </c>
       <c r="AZ9" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>DST</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+        <f t="shared" si="9"/>
+        <v>DST</v>
+      </c>
+      <c r="BA9" s="16">
+        <f t="shared" si="10"/>
+        <v>43.129999999999995</v>
+      </c>
+      <c r="BB9" s="16">
+        <f t="shared" si="11"/>
+        <v>22.614999999999995</v>
+      </c>
+      <c r="BC9" s="16">
+        <f t="shared" si="12"/>
+        <v>20.515000000000015</v>
+      </c>
+      <c r="BD9" s="16">
+        <f t="shared" si="13"/>
+        <v>21.943299999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="H10" s="13"/>
       <c r="I10" s="9"/>
       <c r="J10" s="10"/>
@@ -13291,7 +13714,7 @@
       <c r="AR10" s="10"/>
       <c r="AS10" s="10"/>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -13334,8 +13757,24 @@
       <c r="AQ11" s="10"/>
       <c r="AR11" s="10"/>
       <c r="AS11" s="10"/>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA11" s="16">
+        <f>MAX(BA3:BA9)</f>
+        <v>124.72000000000003</v>
+      </c>
+      <c r="BB11" s="16">
+        <f>MAX(BB3:BB9)</f>
+        <v>46.242999999999995</v>
+      </c>
+      <c r="BC11" s="16">
+        <f>MAX(BC3:BC9)</f>
+        <v>109.75</v>
+      </c>
+      <c r="BD11" s="16">
+        <f>MAX(BD3:BD9)</f>
+        <v>37.569100000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="I12" s="13"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -13374,7 +13813,7 @@
       <c r="AR12" s="10"/>
       <c r="AS12" s="10"/>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="I13" s="13"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -13413,17 +13852,17 @@
       <c r="AR13" s="10"/>
       <c r="AS13" s="10"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="Q14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="Q15" s="11"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>

</xml_diff>